<commit_message>
Update xlsx template to be explicit on segment vs value comparison
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/AutomatedValidationTemplate.xlsx
+++ b/data/human/adult/validation/Scenarios/AutomatedValidationTemplate.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="88">
   <si>
     <t xml:space="preserve">Scenario Name</t>
   </si>
@@ -107,19 +107,19 @@
            "Dyspnea": { "Severity": { "Scalar0To1": { "Value": 1.0 } } } }} ,</t>
   </si>
   <si>
-    <t xml:space="preserve">Target</t>
+    <t xml:space="preserve">Comparison Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison Segment/Value</t>
   </si>
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Comparison Segment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patient</t>
   </si>
   <si>
-    <t xml:space="preserve">equalTo 25</t>
+    <t xml:space="preserve">equalToValue</t>
   </si>
   <si>
     <t xml:space="preserve">veenhuis2023validation</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">unitless</t>
   </si>
   <si>
-    <t xml:space="preserve">greaterThan 50</t>
+    <t xml:space="preserve">greaterThanValue</t>
   </si>
   <si>
     <t xml:space="preserve">Environment</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">L/cmH2O</t>
   </si>
   <si>
-    <t xml:space="preserve">lessThan 100</t>
+    <t xml:space="preserve">lessThanValue</t>
   </si>
   <si>
     <t xml:space="preserve">Action</t>
@@ -149,7 +149,7 @@
     <t xml:space="preserve">cmH2O s/mL</t>
   </si>
   <si>
-    <t xml:space="preserve">Increase</t>
+    <t xml:space="preserve">trendsToValue</t>
   </si>
   <si>
     <t xml:space="preserve">ActionCmpt</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">ActionName-CmptName-Property</t>
   </si>
   <si>
-    <t xml:space="preserve">Decrease</t>
+    <t xml:space="preserve">equalToSegment</t>
   </si>
   <si>
     <t xml:space="preserve">ActionSub</t>
@@ -167,31 +167,46 @@
     <t xml:space="preserve">ActionName-SubName-Property</t>
   </si>
   <si>
+    <t xml:space="preserve">greaterThanSegment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GasCompartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CmptName-Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lessThanSegment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CmptName-SubName-Property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trendsToSegment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LiquidCompartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range</t>
+  </si>
+  <si>
     <t xml:space="preserve">[20,54]</t>
   </si>
   <si>
-    <t xml:space="preserve">GasCompartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CmptName-Property</t>
+    <t xml:space="preserve">mmHg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notValidating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThermalCompartment</t>
   </si>
   <si>
     <t xml:space="preserve">tbd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CmptName-SubName-Property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiquidCompartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmHg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ThermalCompartment</t>
   </si>
   <si>
     <t xml:space="preserve">TissueCompartment</t>
@@ -290,7 +305,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -322,6 +337,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -350,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -545,6 +567,13 @@
       <right/>
       <top style="medium"/>
       <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -628,11 +657,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,10 +734,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -781,6 +806,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -793,7 +822,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -813,15 +842,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -833,27 +858,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -861,16 +890,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -966,7 +999,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1070,80 +1103,80 @@
       <c r="B6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="25" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="25" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="24" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="25" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" s="10" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="31" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="n">
+      <c r="A12" s="33" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1159,13 +1192,13 @@
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="37" t="s">
@@ -1174,16 +1207,16 @@
       <c r="F13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
         <v>28</v>
       </c>
@@ -1196,15 +1229,15 @@
       <c r="D14" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="40" t="n">
-        <v>1</v>
+      <c r="E14" s="40" t="n">
+        <v>25</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="G14" s="41"/>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
@@ -1217,15 +1250,15 @@
       <c r="D15" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="40" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="45"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="42" t="s">
         <v>33</v>
       </c>
@@ -1238,15 +1271,15 @@
       <c r="D16" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="40" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="45"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="42" t="s">
         <v>36</v>
       </c>
@@ -1256,18 +1289,18 @@
       <c r="C17" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="46"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="40" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="45"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="42" t="s">
         <v>40</v>
       </c>
@@ -1280,15 +1313,15 @@
       <c r="D18" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="45" t="n">
+      <c r="E18" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="46"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="45"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="42" t="s">
         <v>43</v>
       </c>
@@ -1301,15 +1334,15 @@
       <c r="D19" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="45"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="42" t="s">
         <v>46</v>
       </c>
@@ -1319,18 +1352,18 @@
       <c r="C20" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="46"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="45"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="47" t="s">
         <v>46</v>
       </c>
@@ -1341,145 +1374,143 @@
         <v>31</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="46"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="E21" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="45"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="45"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="47" t="s">
         <v>51</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="46"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="47" t="s">
-        <v>50</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="46"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="45"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="50" t="s">
+        <v>57</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E24" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G24" s="50"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="49" t="s">
-        <v>54</v>
+      <c r="F24" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="51"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="50" t="s">
+        <v>59</v>
       </c>
       <c r="B25" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E25" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="50"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="49" t="s">
+      <c r="F25" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="51"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="45" t="n">
+      <c r="D26" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G26" s="50"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="49" t="s">
-        <v>57</v>
+      <c r="F26" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="51"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="50" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E27" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G27" s="50"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="49" t="s">
-        <v>58</v>
+      <c r="F27" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="51"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="50" t="s">
+        <v>63</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>17</v>
@@ -1488,19 +1519,19 @@
         <v>31</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E28" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G28" s="50"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="49" t="s">
-        <v>59</v>
+      <c r="F28" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="51"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="50" t="s">
+        <v>64</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>17</v>
@@ -1509,19 +1540,19 @@
         <v>31</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E29" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="50"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49" t="s">
-        <v>60</v>
+      <c r="F29" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="51"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="50" t="s">
+        <v>65</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>17</v>
@@ -1530,19 +1561,19 @@
         <v>31</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E30" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G30" s="50"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="49" t="s">
-        <v>61</v>
+      <c r="F30" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="51"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="50" t="s">
+        <v>66</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>17</v>
@@ -1551,63 +1582,63 @@
         <v>31</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E31" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="50"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="52" t="s">
+      <c r="F31" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="51"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="55" t="n">
+      <c r="D32" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G32" s="50"/>
+      <c r="F32" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="51"/>
     </row>
     <row r="33" s="10" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="31" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="56" t="n">
         <v>2</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C34" s="57"/>
       <c r="D34" s="57"/>
@@ -1648,7 +1679,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1672,7 +1703,7 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
@@ -1683,11 +1714,11 @@
     </row>
     <row r="2" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="59" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D2" s="59"/>
       <c r="E2" s="4" t="s">
@@ -1721,7 +1752,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,80 +1781,80 @@
       <c r="B6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="25" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="24" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="25" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="24" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" s="10" customFormat="true" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="25" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" s="10" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="31" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="n">
+      <c r="A12" s="33" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1839,13 +1870,13 @@
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="37" t="s">
@@ -1854,16 +1885,16 @@
       <c r="F13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="32"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
         <v>28</v>
       </c>
@@ -1876,15 +1907,16 @@
       <c r="D14" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="40" t="n">
-        <v>1</v>
+      <c r="E14" s="40" t="n">
+        <v>25</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="G14" s="41"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
@@ -1897,15 +1929,16 @@
       <c r="D15" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="40" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="45"/>
+      <c r="I15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="42" t="s">
         <v>33</v>
       </c>
@@ -1918,15 +1951,16 @@
       <c r="D16" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="40" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="45"/>
+      <c r="I16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="42" t="s">
         <v>36</v>
       </c>
@@ -1936,18 +1970,19 @@
       <c r="C17" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="46"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="40" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="45"/>
+      <c r="I17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="42" t="s">
         <v>40</v>
       </c>
@@ -1960,15 +1995,16 @@
       <c r="D18" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="45" t="n">
+      <c r="E18" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="46"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="I18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="42" t="s">
         <v>43</v>
       </c>
@@ -1981,15 +2017,16 @@
       <c r="D19" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="45"/>
+      <c r="I19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="42" t="s">
         <v>46</v>
       </c>
@@ -1999,18 +2036,19 @@
       <c r="C20" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="46"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="45"/>
+      <c r="I20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="47" t="s">
         <v>46</v>
       </c>
@@ -2021,145 +2059,150 @@
         <v>31</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="46"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="E21" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="45"/>
+      <c r="I21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="I22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="47" t="s">
         <v>51</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="46"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="47" t="s">
-        <v>50</v>
       </c>
       <c r="B23" s="48" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="46"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="I23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="50" t="s">
+        <v>57</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E24" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G24" s="50"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="49" t="s">
-        <v>54</v>
+      <c r="F24" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="51"/>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="50" t="s">
+        <v>59</v>
       </c>
       <c r="B25" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E25" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="50"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="49" t="s">
+      <c r="F25" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="51"/>
+      <c r="I25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="45" t="n">
+      <c r="D26" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G26" s="50"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="49" t="s">
-        <v>57</v>
+      <c r="F26" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="51"/>
+      <c r="I26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="50" t="s">
+        <v>62</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E27" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G27" s="50"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="49" t="s">
-        <v>58</v>
+      <c r="F27" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="51"/>
+      <c r="I27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="50" t="s">
+        <v>63</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>17</v>
@@ -2168,19 +2211,20 @@
         <v>31</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E28" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G28" s="50"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="49" t="s">
-        <v>59</v>
+      <c r="F28" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="51"/>
+      <c r="I28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="50" t="s">
+        <v>64</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>17</v>
@@ -2189,19 +2233,20 @@
         <v>31</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E29" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="50"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="49" t="s">
-        <v>60</v>
+      <c r="F29" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="51"/>
+      <c r="I29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="50" t="s">
+        <v>65</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>17</v>
@@ -2210,19 +2255,20 @@
         <v>31</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E30" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G30" s="50"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="49" t="s">
-        <v>61</v>
+      <c r="F30" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="51"/>
+      <c r="I30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="50" t="s">
+        <v>66</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>17</v>
@@ -2231,63 +2277,65 @@
         <v>31</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="45" t="n">
+        <v>58</v>
+      </c>
+      <c r="E31" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="50"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="52" t="s">
+      <c r="F31" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="51"/>
+      <c r="I31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="55" t="n">
+      <c r="D32" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="G32" s="50"/>
+      <c r="F32" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="51"/>
+      <c r="I32" s="0"/>
     </row>
     <row r="33" s="10" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="31" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="53" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="56" t="n">
         <v>2</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C34" s="57"/>
       <c r="D34" s="57"/>
@@ -2337,175 +2385,175 @@
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="60" t="s">
-        <v>68</v>
+      <c r="B2" s="61" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="61" t="s">
-        <v>69</v>
+      <c r="B3" s="62" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="61" t="s">
-        <v>70</v>
+      <c r="B4" s="62" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="61" t="s">
-        <v>71</v>
+      <c r="B5" s="62" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="61" t="s">
-        <v>72</v>
+      <c r="B6" s="62" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="61" t="s">
-        <v>73</v>
+      <c r="C7" s="62" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="61" t="s">
-        <v>74</v>
+      <c r="C8" s="62" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="61" t="s">
-        <v>75</v>
+      <c r="B9" s="62" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="61" t="s">
-        <v>76</v>
+      <c r="B10" s="62" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="61" t="s">
-        <v>77</v>
+      <c r="C11" s="62" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="61" t="s">
-        <v>78</v>
+      <c r="C12" s="62" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="61" t="s">
-        <v>79</v>
+      <c r="C13" s="62" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="61" t="s">
-        <v>80</v>
+      <c r="C14" s="62" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="60" t="s">
-        <v>81</v>
+      <c r="B19" s="61" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="61" t="s">
-        <v>82</v>
+      <c r="B20" s="62" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="62"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="62"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="62"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="62"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="62"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>